<commit_message>
Completing required methods in Account Relations API -- in progress (Build 338)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint19Plan.xlsx
+++ b/doc/Planning/Sprint19Plan.xlsx
@@ -13,9 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Week 1" sheetId="3" r:id="rId2"/>
-    <sheet name="Week 2" sheetId="4" r:id="rId3"/>
-    <sheet name="Week 3" sheetId="5" r:id="rId4"/>
+    <sheet name="Week 1" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="Week 2" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="Week 3" sheetId="5" state="hidden" r:id="rId4"/>
     <sheet name="Comments" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -85,9 +85,6 @@
     <t>انتخاب شعبه شرکت انتخاب شده از نمای درختی شعبه ها هنگام ورود به برنامه</t>
   </si>
   <si>
-    <t>پیش بینی هفته اول اسپرینت 18</t>
-  </si>
-  <si>
     <t>پیش بینی هفته دوم اسپرینت 18</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>نگهداری و استفاده از Cache برای خواندن زیرمجموعه ای از اطلاعات در برنامه</t>
+  </si>
+  <si>
+    <t>پیش بینی هفته اول اسپرینت 19</t>
   </si>
 </sst>
 </file>
@@ -1374,7 +1374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -1390,7 +1390,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1416,7 +1416,7 @@
     <row r="3" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
@@ -1428,7 +1428,7 @@
     <row r="4" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5">
         <v>1</v>
@@ -1440,7 +1440,7 @@
     <row r="5" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -1476,7 +1476,7 @@
     <row r="8" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
@@ -1488,7 +1488,7 @@
     <row r="9" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="5">
         <v>1</v>
@@ -1500,7 +1500,7 @@
     <row r="10" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1512,7 +1512,7 @@
     <row r="11" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
@@ -1524,7 +1524,7 @@
     <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="5">
         <v>1</v>
@@ -1536,7 +1536,7 @@
     <row r="13" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -1548,7 +1548,7 @@
     <row r="14" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -1560,7 +1560,7 @@
     <row r="15" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
@@ -1572,7 +1572,7 @@
     <row r="16" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -1584,7 +1584,7 @@
     <row r="17" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
@@ -1592,13 +1592,13 @@
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
       <c r="F17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
@@ -1606,13 +1606,13 @@
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
@@ -1624,7 +1624,7 @@
     <row r="20" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -1636,7 +1636,7 @@
     <row r="21" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
@@ -1648,7 +1648,7 @@
     <row r="22" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
@@ -1695,7 +1695,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1710,7 +1710,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1956,7 +1956,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2201,7 +2201,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated backlog for Sprint 19
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint19Plan.xlsx
+++ b/doc/Planning/Sprint19Plan.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -155,6 +155,21 @@
   </si>
   <si>
     <t>پیش بینی هفته اول اسپرینت 19</t>
+  </si>
+  <si>
+    <t>فیلتر لیست ها بر اساس کد یا نام در سرویس وب</t>
+  </si>
+  <si>
+    <t>رفع باگ : ایجاد رکورد اضافی در گرید فرزند</t>
+  </si>
+  <si>
+    <t>رفع باگ : مشکل نمایشی در گرید پس از ایجاد رکورد زیرمجموعه</t>
+  </si>
+  <si>
+    <t>رفع باگ : نمایش رکورد والد در فرم ویرایش</t>
+  </si>
+  <si>
+    <t>رفع باگ : مشکل نمایشی منوهای چند سطحی در موبایل و تبلت</t>
   </si>
 </sst>
 </file>
@@ -251,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -288,6 +303,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1038,8 +1056,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F24" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
-  <autoFilter ref="A2:F24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F29" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+  <autoFilter ref="A2:F29"/>
   <tableColumns count="6">
     <tableColumn id="1" name="هدف کاری" dataDxfId="44"/>
     <tableColumn id="2" name="قابلیت" dataDxfId="43"/>
@@ -1372,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1536,7 +1554,7 @@
     <row r="13" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="4" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C13" s="5">
         <v>1</v>
@@ -1548,7 +1566,7 @@
     <row r="14" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="5">
         <v>1</v>
@@ -1560,7 +1578,7 @@
     <row r="15" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
@@ -1572,7 +1590,7 @@
     <row r="16" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -1584,21 +1602,19 @@
     <row r="17" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="5">
         <v>1</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="5">
         <v>1</v>
@@ -1606,25 +1622,27 @@
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C19" s="5">
         <v>1</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C20" s="5">
         <v>1</v>
@@ -1636,7 +1654,7 @@
     <row r="21" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C21" s="5">
         <v>1</v>
@@ -1648,7 +1666,7 @@
     <row r="22" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
@@ -1659,26 +1677,86 @@
     </row>
     <row r="23" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
+      <c r="B23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="4"/>
     </row>
+    <row r="25" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="4"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C29">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E29">
       <formula1>"هفته اول,هفته دوم,هفته سوم,هفته های بعد"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>